<commit_message>
Modifica a file empowerment
</commit_message>
<xml_diff>
--- a/Assignment_1/QuestionariUtenti.xlsx
+++ b/Assignment_1/QuestionariUtenti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giaci/Desktop/IUM Progetto/Assignment_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giaci/Documents/GitHub/ProgettoIUM/Assignment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1AA1C0-7524-F54C-AC63-E063D0F0E3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C278C021-525B-3D48-969F-31C59626305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="980" windowWidth="29480" windowHeight="18520" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="4640" windowWidth="23920" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BEHAVIOURABILITY" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="86">
   <si>
     <t>Decision Making</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>Legenda</t>
-  </si>
-  <si>
-    <t>SE = Self-Efficacy</t>
-  </si>
-  <si>
-    <t>K&amp;S = Knowledge &amp; Skills</t>
   </si>
   <si>
     <t>PC = Personal Control</t>
@@ -301,6 +295,21 @@
   </si>
   <si>
     <t>Task T5 &lt;Adesione ad un evento&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE = Self-Efficacy = capacitàù  di una persona di portsi degli obiettivi in maniera chiara e raggiungerli secondo precisi tempi e strategie </t>
+  </si>
+  <si>
+    <t>K&amp;S = Knowledge &amp; Skills  = conoscenze e competenze</t>
+  </si>
+  <si>
+    <t>Decision Making  = abilità nella scelta della migliore soluzione possibile tra quelle disponibili</t>
+  </si>
+  <si>
+    <t>Self-Management = Capacità di gestire se stessi in ambito lavorativo</t>
+  </si>
+  <si>
+    <t>Engagement = quanto si è coivolti in una operazione</t>
   </si>
 </sst>
 </file>
@@ -806,9 +815,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,11 +845,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17" t="s">
@@ -856,7 +865,7 @@
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>4</v>
@@ -864,11 +873,11 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
@@ -877,7 +886,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -888,11 +897,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17" t="s">
@@ -923,22 +932,37 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
@@ -970,30 +994,30 @@
   <sheetData>
     <row r="1" spans="1:9" ht="45" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -1005,7 +1029,7 @@
     <row r="3" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1016,16 +1040,16 @@
     </row>
     <row r="4" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17">
@@ -1034,14 +1058,14 @@
     </row>
     <row r="5" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -1053,7 +1077,7 @@
     <row r="6" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1064,13 +1088,13 @@
     </row>
     <row r="7" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -1083,7 +1107,7 @@
     </row>
     <row r="8" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -1095,7 +1119,7 @@
     <row r="9" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -1106,16 +1130,16 @@
     </row>
     <row r="10" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
@@ -1124,16 +1148,16 @@
     </row>
     <row r="11" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
@@ -1142,13 +1166,13 @@
     </row>
     <row r="12" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -1161,7 +1185,7 @@
     <row r="13" spans="1:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1172,16 +1196,16 @@
     </row>
     <row r="14" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17">
@@ -1190,15 +1214,15 @@
     </row>
     <row r="15" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -1209,7 +1233,7 @@
     <row r="16" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -1220,14 +1244,14 @@
     </row>
     <row r="17" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -1239,17 +1263,17 @@
     </row>
     <row r="18" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18" s="17">
         <v>5</v>
@@ -1257,7 +1281,7 @@
     </row>
     <row r="19" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1269,7 +1293,7 @@
     <row r="20" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -1280,13 +1304,13 @@
     </row>
     <row r="21" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1298,15 +1322,15 @@
     </row>
     <row r="22" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -1317,7 +1341,7 @@
     <row r="23" spans="1:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -1328,14 +1352,14 @@
     </row>
     <row r="24" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -1346,15 +1370,15 @@
     </row>
     <row r="25" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -1364,7 +1388,7 @@
     </row>
     <row r="26" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -1376,7 +1400,7 @@
     <row r="27" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -1388,16 +1412,16 @@
     </row>
     <row r="28" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
@@ -1406,17 +1430,17 @@
     </row>
     <row r="29" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H29" s="17">
         <v>5</v>
@@ -1424,7 +1448,7 @@
     </row>
     <row r="30" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -1436,7 +1460,7 @@
     <row r="31" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -1447,17 +1471,17 @@
     </row>
     <row r="32" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H32" s="17">
         <v>5</v>
@@ -1465,13 +1489,13 @@
     </row>
     <row r="33" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -1484,7 +1508,7 @@
     <row r="34" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -1495,17 +1519,17 @@
     </row>
     <row r="35" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H35" s="17">
         <v>5</v>
@@ -1513,17 +1537,17 @@
     </row>
     <row r="36" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H36" s="17">
         <v>5</v>
@@ -1700,47 +1724,47 @@
   <sheetData>
     <row r="1" spans="1:9" ht="45" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1748,13 +1772,13 @@
     </row>
     <row r="5" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1763,18 +1787,18 @@
     <row r="6" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -1783,24 +1807,24 @@
     </row>
     <row r="8" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -1808,13 +1832,13 @@
     </row>
     <row r="11" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -1822,13 +1846,13 @@
     </row>
     <row r="12" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -1837,18 +1861,18 @@
     <row r="13" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1856,13 +1880,13 @@
     </row>
     <row r="15" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1871,18 +1895,18 @@
     <row r="16" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -1890,13 +1914,13 @@
     </row>
     <row r="18" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -1905,24 +1929,24 @@
     </row>
     <row r="19" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1930,13 +1954,13 @@
     </row>
     <row r="22" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1945,18 +1969,18 @@
     <row r="23" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1964,13 +1988,13 @@
     </row>
     <row r="25" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1978,24 +2002,24 @@
     </row>
     <row r="26" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -2004,13 +2028,13 @@
     </row>
     <row r="29" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -2018,24 +2042,24 @@
     </row>
     <row r="30" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -2043,13 +2067,13 @@
     </row>
     <row r="33" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H33">
         <v>3</v>
@@ -2058,18 +2082,18 @@
     <row r="34" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H35">
         <v>4</v>
@@ -2077,13 +2101,13 @@
     </row>
     <row r="36" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H36">
         <v>4</v>
@@ -2129,47 +2153,47 @@
   <sheetData>
     <row r="1" spans="1:9" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="7">
         <v>3</v>
@@ -2177,13 +2201,13 @@
     </row>
     <row r="5" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
@@ -2192,18 +2216,18 @@
     <row r="6" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7" s="7">
         <v>4</v>
@@ -2212,24 +2236,24 @@
     </row>
     <row r="8" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10" s="7">
         <v>4</v>
@@ -2237,13 +2261,13 @@
     </row>
     <row r="11" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11" s="7">
         <v>4</v>
@@ -2251,13 +2275,13 @@
     </row>
     <row r="12" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12" s="7">
         <v>3</v>
@@ -2266,18 +2290,18 @@
     <row r="13" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H14" s="7">
         <v>4</v>
@@ -2285,13 +2309,13 @@
     </row>
     <row r="15" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H15" s="7">
         <v>3</v>
@@ -2300,18 +2324,18 @@
     <row r="16" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H17" s="7">
         <v>5</v>
@@ -2319,13 +2343,13 @@
     </row>
     <row r="18" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18" s="7">
         <v>5</v>
@@ -2334,24 +2358,24 @@
     </row>
     <row r="19" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H21" s="7">
         <v>2</v>
@@ -2359,13 +2383,13 @@
     </row>
     <row r="22" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H22" s="7">
         <v>2</v>
@@ -2374,18 +2398,18 @@
     <row r="23" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H24" s="7">
         <v>2</v>
@@ -2393,13 +2417,13 @@
     </row>
     <row r="25" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H25" s="7">
         <v>2</v>
@@ -2407,24 +2431,24 @@
     </row>
     <row r="26" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H28" s="7">
         <v>4</v>
@@ -2433,13 +2457,13 @@
     </row>
     <row r="29" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H29" s="7">
         <v>3</v>
@@ -2447,24 +2471,24 @@
     </row>
     <row r="30" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H32" s="7">
         <v>4</v>
@@ -2472,13 +2496,13 @@
     </row>
     <row r="33" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H33" s="7">
         <v>3</v>
@@ -2487,18 +2511,18 @@
     <row r="34" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H35" s="7">
         <v>4</v>
@@ -2506,13 +2530,13 @@
     </row>
     <row r="36" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H36" s="7">
         <v>3</v>
@@ -2574,29 +2598,29 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="14">
         <f>AVERAGE(C4:C5)</f>
@@ -2605,10 +2629,10 @@
     </row>
     <row r="4" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="10">
         <f>AVERAGE(Quest.Utente1!H4,Quest.Utente2!H4,Quest.Utente3!H4)</f>
@@ -2617,10 +2641,10 @@
     </row>
     <row r="5" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="10">
         <f>AVERAGE(Quest.Utente1!H5,Quest.Utente2!H5,Quest.Utente3!H5)</f>
@@ -2630,10 +2654,10 @@
     <row r="6" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="14">
         <f>AVERAGE(C7)</f>
@@ -2642,10 +2666,10 @@
     </row>
     <row r="7" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <f>AVERAGE(Quest.Utente1!H7,Quest.Utente2!H7,Quest.Utente3!H7)</f>
@@ -2654,18 +2678,18 @@
     </row>
     <row r="8" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="14">
         <f>AVERAGE(C10:C12)</f>
@@ -2674,10 +2698,10 @@
     </row>
     <row r="10" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="10">
         <f>AVERAGE(Quest.Utente1!H10,Quest.Utente2!H10,Quest.Utente3!H10)</f>
@@ -2686,10 +2710,10 @@
     </row>
     <row r="11" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="10">
         <f>AVERAGE(Quest.Utente1!H11,Quest.Utente2!H11,Quest.Utente3!H11)</f>
@@ -2698,10 +2722,10 @@
     </row>
     <row r="12" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="10">
         <f>AVERAGE(Quest.Utente1!H12,Quest.Utente2!H12,Quest.Utente3!H12)</f>
@@ -2711,11 +2735,11 @@
     <row r="13" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="14">
         <f>AVERAGE(C14:C15)</f>
@@ -2724,10 +2748,10 @@
     </row>
     <row r="14" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="10">
         <f>AVERAGE(Quest.Utente1!H14,Quest.Utente2!H14,Quest.Utente3!H14)</f>
@@ -2736,10 +2760,10 @@
     </row>
     <row r="15" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="10">
         <f>AVERAGE(Quest.Utente1!H15,Quest.Utente2!H15,Quest.Utente3!H15)</f>
@@ -2749,10 +2773,10 @@
     <row r="16" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="14">
         <f>AVERAGE(C17:C18)</f>
@@ -2761,10 +2785,10 @@
     </row>
     <row r="17" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="10">
         <f>AVERAGE(Quest.Utente1!H17,Quest.Utente2!H17,Quest.Utente3!H17)</f>
@@ -2773,10 +2797,10 @@
     </row>
     <row r="18" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="10">
         <f>AVERAGE(Quest.Utente1!H18,Quest.Utente2!H18,Quest.Utente3!H18)</f>
@@ -2785,18 +2809,18 @@
     </row>
     <row r="19" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E20" s="18">
         <f>AVERAGE(C21:C22)</f>
@@ -2805,10 +2829,10 @@
     </row>
     <row r="21" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="10">
         <f>AVERAGE(Quest.Utente1!H21,Quest.Utente2!H21,Quest.Utente3!H21)</f>
@@ -2817,10 +2841,10 @@
     </row>
     <row r="22" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="10">
         <f>AVERAGE(Quest.Utente1!H22,Quest.Utente2!H22,Quest.Utente3!H22)</f>
@@ -2830,11 +2854,11 @@
     <row r="23" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="18">
         <f>AVERAGE(C24:C25)</f>
@@ -2843,10 +2867,10 @@
     </row>
     <row r="24" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="10">
         <f>AVERAGE(Quest.Utente1!H24,Quest.Utente2!H24,Quest.Utente3!H24)</f>
@@ -2855,10 +2879,10 @@
     </row>
     <row r="25" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="10">
         <f>AVERAGE(Quest.Utente1!H25,Quest.Utente2!H25,Quest.Utente3!H25)</f>
@@ -2867,16 +2891,16 @@
     </row>
     <row r="26" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E27" s="18">
         <f>AVERAGE(C28:C29)</f>
@@ -2885,10 +2909,10 @@
     </row>
     <row r="28" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="10">
         <f>AVERAGE(Quest.Utente1!H28,Quest.Utente2!H28,Quest.Utente3!H28)</f>
@@ -2897,10 +2921,10 @@
     </row>
     <row r="29" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="10">
         <f>AVERAGE(Quest.Utente1!H29,Quest.Utente2!H29,Quest.Utente3!H29)</f>
@@ -2909,16 +2933,16 @@
     </row>
     <row r="30" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E31" s="18">
         <f>AVERAGE(C32:C33)</f>
@@ -2927,10 +2951,10 @@
     </row>
     <row r="32" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="10">
         <f>AVERAGE(Quest.Utente1!H32,Quest.Utente2!H32,Quest.Utente3!H32)</f>
@@ -2939,10 +2963,10 @@
     </row>
     <row r="33" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="10">
         <f>AVERAGE(Quest.Utente1!H33,Quest.Utente2!H33,Quest.Utente3!H33)</f>
@@ -2952,10 +2976,10 @@
     <row r="34" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E34" s="18">
         <f>AVERAGE(C35:C36)</f>
@@ -2964,10 +2988,10 @@
     </row>
     <row r="35" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="10">
         <f>AVERAGE(Quest.Utente1!H35,Quest.Utente2!H35,Quest.Utente3!H35)</f>
@@ -2976,10 +3000,10 @@
     </row>
     <row r="36" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="10">
         <f>AVERAGE(Quest.Utente1!H36,Quest.Utente2!H36,Quest.Utente3!H36)</f>
@@ -2996,7 +3020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3007,24 +3031,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="15">
         <f>MEDIE!E3</f>
@@ -3039,7 +3063,7 @@
     </row>
     <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="22">
@@ -3057,7 +3081,7 @@
     </row>
     <row r="4" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="15">
         <f>MEDIE!E20</f>
@@ -3072,7 +3096,7 @@
     </row>
     <row r="5" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="16"/>
@@ -3084,7 +3108,7 @@
     </row>
     <row r="6" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="19">
         <f>MEDIE!E31</f>

</xml_diff>